<commit_message>
added data generation functionality
</commit_message>
<xml_diff>
--- a/src/test/Test.xlsx
+++ b/src/test/Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28200" windowHeight="14985"/>
+    <workbookView windowWidth="28695" windowHeight="14985"/>
   </bookViews>
   <sheets>
     <sheet name="smoke" sheetId="1" r:id="rId1"/>
@@ -82,19 +82,19 @@
     <t>SendWeatherForecast</t>
   </si>
   <si>
-    <t>https://ua.sinoptik.ua/</t>
-  </si>
-  <si>
-    <t>Ternopil</t>
-  </si>
-  <si>
-    <t>https://mail.ukr.net</t>
-  </si>
-  <si>
-    <t>autotests</t>
-  </si>
-  <si>
-    <t>1234567891</t>
+    <t>MD_COMMON_LINKS_SINOPTIKURL</t>
+  </si>
+  <si>
+    <t>MD_COMMON_VALIDDATA_TERNOPILCITY</t>
+  </si>
+  <si>
+    <t>MD_COMMON_LINKS_UKRNETMAILURL</t>
+  </si>
+  <si>
+    <t>MD_COMMON_CREDENTIALS_UKRNETUSER</t>
+  </si>
+  <si>
+    <t>MD_COMMON_CREDENTIALS_UKRNETPASSWORD</t>
   </si>
   <si>
     <t>belphegor89@ukr.net</t>
@@ -105,12 +105,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,12 +134,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -147,7 +155,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -161,44 +192,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -209,6 +202,21 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -223,13 +231,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -238,6 +239,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -245,6 +261,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,36 +292,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -305,73 +313,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,108 +494,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -514,6 +522,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -533,21 +565,21 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -556,8 +588,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -587,34 +619,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -632,38 +640,38 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -672,88 +680,88 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -761,9 +769,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1086,20 +1094,19 @@
   <sheetPr/>
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="26.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="21.7142857142857" customWidth="1"/>
-    <col min="3" max="3" width="12.5714285714286" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="12.5714285714286" customWidth="1"/>
-    <col min="6" max="6" width="15.8380952380952" customWidth="1"/>
+    <col min="2" max="2" width="36.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="43.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="40.4285714285714" customWidth="1"/>
+    <col min="5" max="6" width="44" customWidth="1"/>
     <col min="7" max="7" width="20.7142857142857" customWidth="1"/>
     <col min="8" max="10" width="12.5714285714286" customWidth="1"/>
     <col min="11" max="21" width="13.8571428571429" customWidth="1"/>
@@ -1178,22 +1185,22 @@
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -1210,9 +1217,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://ua.sinoptik.ua/"/>
-    <hyperlink ref="D2" r:id="rId2" display="https://mail.ukr.net"/>
-    <hyperlink ref="G2" r:id="rId3" display="belphegor89@ukr.net"/>
+    <hyperlink ref="G2" r:id="rId1" display="belphegor89@ukr.net" tooltip="mailto:belphegor89@ukr.net"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>